<commit_message>
Mise à jour journal de travail Jonny
</commit_message>
<xml_diff>
--- a/Documents/Journal de travail - Module 2 - Jonny HOFMANN.xlsx
+++ b/Documents/Journal de travail - Module 2 - Jonny HOFMANN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leapp\Documents\projects\app_module_2\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C05F9B-49DD-456B-9AF8-A72D0393BE0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4870AFF-8FF7-471C-AFB2-CFFC6C47F526}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{70D5A45C-33B5-45AC-81A1-24A22F03E0AB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="93">
   <si>
     <t>Date</t>
   </si>
@@ -169,18 +169,12 @@
     <t>Création et structuration de github</t>
   </si>
   <si>
-    <t>Création du .gitignoew</t>
-  </si>
-  <si>
     <t>Corrections sur la base de données</t>
   </si>
   <si>
     <t>Création de scripts supplémentaires pour la BD</t>
   </si>
   <si>
-    <t>Base du DBManager</t>
-  </si>
-  <si>
     <t>Affichage des recettes</t>
   </si>
   <si>
@@ -202,9 +196,6 @@
     <t>1.10.19</t>
   </si>
   <si>
-    <t>Ajout édition recette</t>
-  </si>
-  <si>
     <t>8.10.19</t>
   </si>
   <si>
@@ -275,6 +266,54 @@
   </si>
   <si>
     <t>11.11.19</t>
+  </si>
+  <si>
+    <t>Création du MCD</t>
+  </si>
+  <si>
+    <t>Généré le code sql et l'appliquer</t>
+  </si>
+  <si>
+    <t>Créer script de données de tests et remplir la BD</t>
+  </si>
+  <si>
+    <t>Création de la planification</t>
+  </si>
+  <si>
+    <t>Création du .gitignore</t>
+  </si>
+  <si>
+    <t>Calculs des heures par taches</t>
+  </si>
+  <si>
+    <t>Se documenter et faire l'interface basic</t>
+  </si>
+  <si>
+    <t>Installation et debugage du connecteur</t>
+  </si>
+  <si>
+    <t>Test et base de la classe DBManager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajout de fonctionnalités </t>
+  </si>
+  <si>
+    <t>commencer l'édition de recette</t>
+  </si>
+  <si>
+    <t>finir l'édition de recette</t>
+  </si>
+  <si>
+    <t>rédaction de la documentation technique</t>
+  </si>
+  <si>
+    <t>Description des fonctions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descriptions des interfaces et fonctionnalités </t>
+  </si>
+  <si>
+    <t>Reste de la documentation technique</t>
   </si>
 </sst>
 </file>
@@ -282,8 +321,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="hh/mm&quot; h&quot;;@"/>
-    <numFmt numFmtId="166" formatCode="[$-100C]dddd\,\ d\.\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+    <numFmt numFmtId="165" formatCode="[$-100C]dddd\,\ d\.\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -337,7 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -355,6 +394,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,19 +410,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <numFmt numFmtId="166" formatCode="[$-100C]dddd\,\ d\.\ mmmm\ yyyy;@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -408,15 +443,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="hh/mm&quot; h&quot;;@"/>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="hh/mm&quot; h&quot;;@"/>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="hh/mm&quot; h&quot;;@"/>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-100C]dddd\,\ d\.\ mmmm\ yyyy;@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -505,35 +544,35 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2D9C452D-B696-49AE-85E7-6BE5689175E8}" name="Date" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{4DDB3066-4F5D-4928-B063-7A79BD8A56C0}" name="Heure début" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{747ABF81-AFD0-4CCC-B0EF-5BD4A67CB89A}" name="Heure fin" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{44C70AFE-3A63-4D7C-BCE2-AFCBE350D7E0}" name="Durée [h]" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{2D9C452D-B696-49AE-85E7-6BE5689175E8}" name="Date" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{4DDB3066-4F5D-4928-B063-7A79BD8A56C0}" name="Heure début" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{747ABF81-AFD0-4CCC-B0EF-5BD4A67CB89A}" name="Heure fin" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{44C70AFE-3A63-4D7C-BCE2-AFCBE350D7E0}" name="Durée [h]" dataDxfId="9">
       <calculatedColumnFormula>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1F44C5F1-9DC7-49FD-BEA5-FE2D51695105}" name="Activité" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{E3A601BE-D1B0-40B4-B4F2-F242918C1B5C}" name="Tâche" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{67E08D0C-328E-45D8-BA0B-9DBA13917780}" name="Description" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{1F44C5F1-9DC7-49FD-BEA5-FE2D51695105}" name="Activité" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{E3A601BE-D1B0-40B4-B4F2-F242918C1B5C}" name="Tâche" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{67E08D0C-328E-45D8-BA0B-9DBA13917780}" name="Description" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CB3D1BC4-5BDF-4BCD-BAA0-E8CB34AE7763}" name="Tableau2" displayName="Tableau2" ref="A1:A5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CB3D1BC4-5BDF-4BCD-BAA0-E8CB34AE7763}" name="Tableau2" displayName="Tableau2" ref="A1:A5" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:A5" xr:uid="{8ED7C11D-9C44-4D9F-99A4-20ECD07A5D1A}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A5344F17-BC94-4BF4-AC3E-A02F10F7FAC9}" name="Tâches" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{A5344F17-BC94-4BF4-AC3E-A02F10F7FAC9}" name="Tâches" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0C3B6CA0-0D10-4751-A9F4-A9C39600A867}" name="Tableau3" displayName="Tableau3" ref="C1:C17" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0C3B6CA0-0D10-4751-A9F4-A9C39600A867}" name="Tableau3" displayName="Tableau3" ref="C1:C17" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="C1:C17" xr:uid="{717E42E2-8607-4B61-8D36-26CE71AFAF3F}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{77F82D2F-438D-46DD-8F1F-526F0524EBB4}" name="Activités" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{77F82D2F-438D-46DD-8F1F-526F0524EBB4}" name="Activités" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -841,8 +880,8 @@
   </sheetPr>
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,24 +894,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -884,11 +923,11 @@
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="8" t="s">
@@ -897,11 +936,11 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="8" t="s">
@@ -910,11 +949,11 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -941,11 +980,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="3">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.43055555555555558</v>
+      </c>
       <c r="D9" s="3">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -955,10 +998,12 @@
       <c r="F9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="3"/>
@@ -972,10 +1017,12 @@
       <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="3"/>
@@ -989,10 +1036,12 @@
       <c r="F11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="3"/>
@@ -1011,7 +1060,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="3"/>
@@ -1025,10 +1074,12 @@
       <c r="F13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="3"/>
@@ -1043,11 +1094,11 @@
         <v>24</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="3"/>
@@ -1061,10 +1112,12 @@
       <c r="F15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="3"/>
@@ -1079,11 +1132,11 @@
         <v>15</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="3"/>
@@ -1098,11 +1151,11 @@
         <v>15</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="3"/>
@@ -1116,10 +1169,12 @@
       <c r="F18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3">
@@ -1139,11 +1194,11 @@
         <v>16</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="3">
@@ -1156,16 +1211,18 @@
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]]</f>
         <v>0.16666666666666669</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>10</v>
+      <c r="E20" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="3">
@@ -1179,15 +1236,17 @@
         <v>0.125</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B22" s="3">
@@ -1201,15 +1260,17 @@
         <v>0.16666666666666669</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="1"/>
+      <c r="G22" s="7" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="3">
@@ -1229,12 +1290,12 @@
         <v>21</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>50</v>
       </c>
       <c r="B24" s="3">
         <v>0.5625</v>
@@ -1253,12 +1314,12 @@
         <v>21</v>
       </c>
       <c r="G24" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>51</v>
       </c>
       <c r="B25" s="3">
         <v>0.70833333333333337</v>
@@ -1276,11 +1337,13 @@
       <c r="F25" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="7"/>
+      <c r="G25" s="7" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>52</v>
+      <c r="A26" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="B26" s="3">
         <v>0.34722222222222227</v>
@@ -1299,12 +1362,12 @@
         <v>21</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>54</v>
+      <c r="A27" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="B27" s="3">
         <v>0.5625</v>
@@ -1323,12 +1386,12 @@
         <v>21</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>56</v>
+      <c r="A28" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="B28" s="3">
         <v>0.54166666666666663</v>
@@ -1346,12 +1409,12 @@
         <v>21</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>58</v>
+      <c r="A29" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="B29" s="3">
         <v>0.54166666666666663</v>
@@ -1370,12 +1433,12 @@
         <v>21</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>60</v>
+      <c r="A30" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="B30" s="3">
         <v>0.54166666666666663</v>
@@ -1394,12 +1457,12 @@
         <v>22</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>62</v>
+      <c r="A31" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="B31" s="3">
         <v>0.34722222222222227</v>
@@ -1418,12 +1481,12 @@
         <v>22</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>64</v>
+      <c r="A32" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="B32" s="3">
         <v>0.54166666666666663</v>
@@ -1442,12 +1505,12 @@
         <v>23</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>65</v>
+      <c r="A33" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="B33" s="3">
         <v>0.54166666666666663</v>
@@ -1466,12 +1529,12 @@
         <v>23</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>67</v>
+      <c r="A34" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="B34" s="3">
         <v>0.75</v>
@@ -1490,12 +1553,12 @@
         <v>23</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>69</v>
+      <c r="A35" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="B35" s="3">
         <v>0.625</v>
@@ -1514,12 +1577,12 @@
         <v>23</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>71</v>
+      <c r="A36" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="B36" s="3">
         <v>0.34722222222222227</v>
@@ -1538,12 +1601,12 @@
         <v>24</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>73</v>
+      <c r="A37" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="B37" s="3">
         <v>0.58333333333333337</v>
@@ -1562,12 +1625,12 @@
         <v>24</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>74</v>
+      <c r="A38" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="B38" s="3">
         <v>0.34722222222222227</v>
@@ -1585,11 +1648,13 @@
       <c r="F38" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G38" s="7"/>
+      <c r="G38" s="7" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>75</v>
+      <c r="A39" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="B39" s="3">
         <v>0.5625</v>
@@ -1607,11 +1672,13 @@
       <c r="F39" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G39" s="7"/>
+      <c r="G39" s="7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>76</v>
+      <c r="A40" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="B40" s="3">
         <v>0.5625</v>
@@ -1632,8 +1699,8 @@
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>77</v>
+      <c r="A41" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="B41" s="3">
         <v>0.75</v>
@@ -1651,11 +1718,13 @@
       <c r="F41" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G41" s="7"/>
+      <c r="G41" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>78</v>
+      <c r="A42" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="B42" s="3">
         <v>0.66666666666666663</v>
@@ -1676,8 +1745,8 @@
       <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>79</v>
+      <c r="A43" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="B43" s="3">
         <v>0.58333333333333337</v>
@@ -1695,10 +1764,12 @@
       <c r="F43" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G43" s="7"/>
+      <c r="G43" s="7" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="10"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>

</xml_diff>